<commit_message>
modificacion de la plantilla
</commit_message>
<xml_diff>
--- a/web_app/public/plantillas/asignaturasPlantilla.xlsx
+++ b/web_app/public/plantillas/asignaturasPlantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFG\TFG-PAP\web_app\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4839EAF4-FAB1-444A-B0E6-970CC12B203D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA157C73-0D40-44F5-BFB1-7BE1A3E04F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>ASIGNATURAS</t>
-  </si>
-  <si>
     <t>Codigo</t>
   </si>
   <si>
@@ -40,6 +37,9 @@
   </si>
   <si>
     <t>Titulacion</t>
+  </si>
+  <si>
+    <t>Curso</t>
   </si>
 </sst>
 </file>
@@ -89,13 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,35 +384,30 @@
     <col min="1" max="4" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D11" s="2"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>